<commit_message>
corrected "cape" in AAT files
</commit_message>
<xml_diff>
--- a/aat_whg-subset.xlsx
+++ b/aat_whg-subset.xlsx
@@ -1981,8 +1981,8 @@
   <dimension ref="A1:H162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4325,7 +4325,7 @@
         <v>300266060</v>
       </c>
       <c r="C118" s="10">
-        <v>300386845</v>
+        <v>300008850</v>
       </c>
       <c r="D118" s="19" t="s">
         <v>348</v>

</xml_diff>